<commit_message>
added Bulk Link functionality
</commit_message>
<xml_diff>
--- a/linkinglogs_file.xlsx
+++ b/linkinglogs_file.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="89">
   <si>
     <t>S.NO</t>
   </si>
@@ -76,151 +76,205 @@
     <t>0</t>
   </si>
   <si>
-    <t>011433153669</t>
-  </si>
-  <si>
-    <t>CAS F94</t>
-  </si>
-  <si>
-    <t>2.85</t>
-  </si>
-  <si>
-    <t>3.51</t>
+    <t>14987563</t>
+  </si>
+  <si>
+    <t>CAS SB42</t>
+  </si>
+  <si>
+    <t>1.17</t>
+  </si>
+  <si>
+    <t>2.99</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>A DELICIOUS SNACK PILLOW DELIGHT</t>
+  </si>
+  <si>
+    <t>DEEP BOT CUMIN PWD (B) 70Z (12)</t>
+  </si>
+  <si>
+    <t>SNACKS</t>
+  </si>
+  <si>
+    <t>7 OZ</t>
+  </si>
+  <si>
+    <t>11:18:21</t>
+  </si>
+  <si>
+    <t>8901719110993</t>
+  </si>
+  <si>
+    <t>CAS SB43</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>PARLE MONACO SNACKS</t>
+  </si>
+  <si>
+    <t>DEEP BOT COR-CUMINPWD (B) 70Z (12)</t>
+  </si>
+  <si>
+    <t>250GM</t>
+  </si>
+  <si>
+    <t>8696132004003</t>
+  </si>
+  <si>
+    <t>CAS SB35</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>3.99</t>
+  </si>
+  <si>
+    <t>SNACKSOFT SUN DRIED FIGS</t>
+  </si>
+  <si>
+    <t>DEEP BOT CORINDERSEED (B) 3. 5 (12)</t>
+  </si>
+  <si>
+    <t>DRYFRUITS</t>
+  </si>
+  <si>
+    <t>16 OZ</t>
+  </si>
+  <si>
+    <t>8904083524274</t>
+  </si>
+  <si>
+    <t>CAS SB15</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>FYVE  ELEMENTS TRADITIONAL SNACKS</t>
+  </si>
+  <si>
+    <t>DEEP BOT CUMIN SEEDS (B) 14OZ (6)</t>
+  </si>
+  <si>
+    <t>GROCERY</t>
+  </si>
+  <si>
+    <t>200G</t>
+  </si>
+  <si>
+    <t>723246293011</t>
+  </si>
+  <si>
+    <t>CAS SB16</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>1.99</t>
+  </si>
+  <si>
+    <t>AMMA SNACKS  ANDHRA</t>
+  </si>
+  <si>
+    <t>DEEP BOT CUMIN. PWD (B) 14OZ (6)</t>
+  </si>
+  <si>
+    <t>200 g</t>
+  </si>
+  <si>
+    <t>8906127360121</t>
+  </si>
+  <si>
+    <t>CAS SB39</t>
+  </si>
+  <si>
+    <t>1.08</t>
+  </si>
+  <si>
+    <t>3.49</t>
+  </si>
+  <si>
+    <t>KERA HAND CRAFTED SNACK</t>
+  </si>
+  <si>
+    <t>DEEP BOT CURRY PWD (B) 5. 30Z (12)</t>
+  </si>
+  <si>
+    <t>627843331117</t>
+  </si>
+  <si>
+    <t>CAS SB37</t>
+  </si>
+  <si>
+    <t>7.70</t>
+  </si>
+  <si>
     <t>YES</t>
   </si>
   <si>
-    <t>DEEP MULTI GRAIN FLOUR</t>
-  </si>
-  <si>
-    <t>DEEP FLO MULTIGRAINFLOUR4LB</t>
-  </si>
-  <si>
-    <t>ATTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10 lb</t>
-  </si>
-  <si>
-    <t>10:37:52</t>
-  </si>
-  <si>
-    <t>788821045096</t>
-  </si>
-  <si>
-    <t>CAS F49</t>
-  </si>
-  <si>
-    <t>1.27</t>
-  </si>
-  <si>
-    <t>1.56</t>
-  </si>
-  <si>
-    <t>SHAN KHALIS HALDEE</t>
-  </si>
-  <si>
-    <t>DEEP FLO SOOJI CORSEFLR 21B (20)</t>
-  </si>
-  <si>
-    <t>SPICES</t>
-  </si>
-  <si>
-    <t>200 G</t>
-  </si>
-  <si>
-    <t>810347001901</t>
-  </si>
-  <si>
-    <t>CAS F78</t>
-  </si>
-  <si>
-    <t>3.44</t>
-  </si>
-  <si>
-    <t>4.23</t>
-  </si>
-  <si>
-    <t>ZAHARAT AL KHALEEJ</t>
-  </si>
-  <si>
-    <t>DEEP FLO ROASTED UPMAMIX4LK (10)</t>
-  </si>
-  <si>
-    <t>RICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>723246297187</t>
-  </si>
-  <si>
-    <t>CAS F48L</t>
-  </si>
-  <si>
-    <t>4.80</t>
-  </si>
-  <si>
-    <t>5.90</t>
-  </si>
-  <si>
-    <t>RICE FLOUR</t>
-  </si>
-  <si>
-    <t>DEEP FLO RICE FLOUR 81B (5)</t>
-  </si>
-  <si>
-    <t>GROCERY</t>
-  </si>
-  <si>
-    <t>10:21:23</t>
-  </si>
-  <si>
-    <t>011433153676</t>
-  </si>
-  <si>
-    <t>CAS F26</t>
-  </si>
-  <si>
-    <t>3.49</t>
-  </si>
-  <si>
-    <t>4.29</t>
-  </si>
-  <si>
-    <t>DEEP FLO RAGI FLOUR 4LBS (10)</t>
-  </si>
-  <si>
-    <t>4 LB</t>
-  </si>
-  <si>
-    <t>123475</t>
-  </si>
-  <si>
-    <t>CAS P75</t>
-  </si>
-  <si>
-    <t>1.57</t>
-  </si>
-  <si>
-    <t>1.93</t>
-  </si>
-  <si>
-    <t>pickle masala</t>
-  </si>
-  <si>
-    <t>DEEP PIC PICKLE MASALA 7OZ (12)</t>
+    <t>REAL SNACKS</t>
+  </si>
+  <si>
+    <t>DEEP BOT GRENCARDAMOM (B) 3. 5 (12)</t>
+  </si>
+  <si>
+    <t>878776005037</t>
+  </si>
+  <si>
+    <t>CAS SB38</t>
+  </si>
+  <si>
+    <t>2.52</t>
+  </si>
+  <si>
+    <t>2.79</t>
+  </si>
+  <si>
+    <t>ANAND GARLIC MIXTURE SNACK MIX</t>
+  </si>
+  <si>
+    <t>DEEP BOT GARAMMASALA (B) 5. (12)</t>
+  </si>
+  <si>
+    <t>400 GM</t>
+  </si>
+  <si>
+    <t>068656021824</t>
+  </si>
+  <si>
+    <t>CAS SB44</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>4.49</t>
+  </si>
+  <si>
+    <t>SHALINI MIXED SAVOURIES SNACK</t>
+  </si>
+  <si>
+    <t>DEEP BOT GARLIC POWDER (B) 14 (6)</t>
+  </si>
+  <si>
+    <t>600 GM</t>
   </si>
   <si>
     <t>VENDOR:chetak</t>
   </si>
   <si>
-    <t>INV #:Deepanshu testing - INV DATE:2022-02-25</t>
+    <t>INV #:996578 - INV DATE:2022-01-27</t>
   </si>
   <si>
     <t>LINKED BY #:deeepanshunayak</t>
@@ -685,7 +739,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:V16"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="10" customWidth="1"/>
@@ -785,7 +839,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>23</v>
@@ -799,32 +853,32 @@
       <c r="J2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="Q2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
@@ -841,52 +895,52 @@
         <v>20</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="S3" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
@@ -903,52 +957,52 @@
         <v>20</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="I4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="8" t="s">
+      <c r="Q4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="R4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="S4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T4" s="8"/>
       <c r="U4" s="8"/>
@@ -965,50 +1019,52 @@
         <v>20</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="H5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="Q5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="8" t="s">
+      <c r="R5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="P5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="R5" s="8"/>
       <c r="S5" s="8" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
@@ -1025,19 +1081,19 @@
         <v>20</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>25</v>
@@ -1045,8 +1101,8 @@
       <c r="J6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>26</v>
+      <c r="K6" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>25</v>
@@ -1058,19 +1114,19 @@
         <v>25</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="P6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="R6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="S6" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="T6" s="8"/>
       <c r="U6" s="8"/>
@@ -1087,19 +1143,19 @@
         <v>20</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>25</v>
@@ -1107,8 +1163,8 @@
       <c r="J7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="9" t="s">
-        <v>26</v>
+      <c r="K7" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>25</v>
@@ -1120,19 +1176,17 @@
         <v>25</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>61</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="R7" s="8"/>
       <c r="S7" s="8" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="T7" s="8"/>
       <c r="U7" s="8"/>
@@ -1149,19 +1203,19 @@
         <v>20</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>25</v>
@@ -1170,7 +1224,7 @@
         <v>25</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>25</v>
@@ -1182,19 +1236,17 @@
         <v>25</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="R8" s="8" t="s">
-        <v>47</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="R8" s="8"/>
       <c r="S8" s="8" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="T8" s="8"/>
       <c r="U8" s="8"/>
@@ -1202,39 +1254,163 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I10" s="10">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="S10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I12" s="10">
         <v>0</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J12" s="11">
         <v>0</v>
       </c>
-      <c r="K10" s="12">
-        <v>7</v>
-      </c>
-      <c r="L10" s="13">
+      <c r="K12" s="12">
+        <v>1</v>
+      </c>
+      <c r="L12" s="13">
         <v>0</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M12" s="14">
         <v>0</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N12" s="15">
         <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>70</v>
+      <c r="A14" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sync products,update inventory and fix some error
</commit_message>
<xml_diff>
--- a/linkinglogs_file.xlsx
+++ b/linkinglogs_file.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="69">
   <si>
     <t>S.NO</t>
   </si>
@@ -64,6 +64,12 @@
     <t>PRICE SAME</t>
   </si>
   <si>
+    <t>Old Qty</t>
+  </si>
+  <si>
+    <t>New Qty</t>
+  </si>
+  <si>
     <t>POS DESCRIPTION</t>
   </si>
   <si>
@@ -82,64 +88,67 @@
     <t>ITEM CODE ERROR</t>
   </si>
   <si>
+    <t>1.40</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>DEEP BOT CUMIN SEEDS (B) 14OZ (6)</t>
+  </si>
+  <si>
+    <t>12:22:12</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>DEEP BOT CUMIN. PWD (B) 14OZ (6)</t>
+  </si>
+  <si>
+    <t>1.66</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
-    <t>011433152334</t>
-  </si>
-  <si>
-    <t>PK 4KP</t>
-  </si>
-  <si>
-    <t>3.29</t>
-  </si>
-  <si>
-    <t/>
+    <t>807522004482</t>
+  </si>
+  <si>
+    <t>CAS SB15</t>
+  </si>
+  <si>
+    <t>1.22</t>
   </si>
   <si>
     <t>YES</t>
   </si>
   <si>
-    <t>2.49</t>
-  </si>
-  <si>
-    <t>METHI PAKORA</t>
-  </si>
-  <si>
-    <t>REENAS CUP-KAJU DRAKSH (18)</t>
-  </si>
-  <si>
-    <t>MISCELLANEOUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>07:40:31</t>
-  </si>
-  <si>
-    <t>5.29</t>
-  </si>
-  <si>
-    <t>REENAS CUP-KESAR PISTA (18)</t>
-  </si>
-  <si>
-    <t>011433114677</t>
-  </si>
-  <si>
-    <t>PK 6ML</t>
-  </si>
-  <si>
-    <t>1.94</t>
-  </si>
-  <si>
-    <t>1.89</t>
-  </si>
-  <si>
-    <t>DEEP FENNEL POWDER</t>
-  </si>
-  <si>
-    <t>REENAS CUP-MALAI KULFI (18)</t>
+    <t>5.99</t>
+  </si>
+  <si>
+    <t>HERBI METHI POWDER</t>
+  </si>
+  <si>
+    <t>HBA</t>
+  </si>
+  <si>
+    <t>198.5 gms</t>
+  </si>
+  <si>
+    <t>011433073196</t>
+  </si>
+  <si>
+    <t>CAS SB16</t>
+  </si>
+  <si>
+    <t>1.52</t>
+  </si>
+  <si>
+    <t>4.81</t>
+  </si>
+  <si>
+    <t>DEEP FENUGREEK SEEDS</t>
   </si>
   <si>
     <t>SPICES</t>
@@ -148,37 +157,64 @@
     <t>7 OZ</t>
   </si>
   <si>
-    <t>011433071192</t>
-  </si>
-  <si>
-    <t>PK 2FK</t>
-  </si>
-  <si>
-    <t>1.22</t>
-  </si>
-  <si>
-    <t>1.57</t>
-  </si>
-  <si>
-    <t>DEEP FENUGREEK SEEDS</t>
-  </si>
-  <si>
-    <t>REENAS FALOODA KULFI - QT (4)</t>
-  </si>
-  <si>
-    <t>14 OZ</t>
-  </si>
-  <si>
-    <t>PK 2KP</t>
-  </si>
-  <si>
-    <t>REENAS KESAR PISTA QT (4)</t>
+    <t>08:13:08</t>
+  </si>
+  <si>
+    <t>894700010434</t>
+  </si>
+  <si>
+    <t>CAS SB43</t>
+  </si>
+  <si>
+    <t>2.32</t>
+  </si>
+  <si>
+    <t>6.83</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>CHOBANI GREEK YOGURT WW PLAIN</t>
+  </si>
+  <si>
+    <t>DEEP BOT COR-CUMINPWD (B) 70Z (12)</t>
+  </si>
+  <si>
+    <t>DIARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">907 gm </t>
+  </si>
+  <si>
+    <t>894700010069</t>
+  </si>
+  <si>
+    <t>CAS SB35</t>
+  </si>
+  <si>
+    <t>1.41</t>
+  </si>
+  <si>
+    <t>1.72</t>
+  </si>
+  <si>
+    <t>CHOBANI GREEK YOGURT PEACH NONFAT</t>
+  </si>
+  <si>
+    <t>DEEP BOT CORINDERSEED (B) 3. 5 (12)</t>
+  </si>
+  <si>
+    <t>FROZENFOOD</t>
+  </si>
+  <si>
+    <t>6 OZ</t>
   </si>
   <si>
     <t>VENDOR:chetak</t>
   </si>
   <si>
-    <t>INV #:996772 - INV DATE:2022-01-28</t>
+    <t>INV #:996578 - INV DATE:2022-01-27</t>
   </si>
   <si>
     <t>LINKED BY #:deeepanshunayak</t>
@@ -271,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -296,9 +332,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -646,7 +680,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:AB16"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="10" customWidth="1"/>
@@ -658,14 +692,14 @@
     <col min="11" max="11" width="15" customWidth="1"/>
     <col min="12" max="15" width="10" customWidth="1"/>
     <col min="16" max="16" width="12" customWidth="1"/>
-    <col min="17" max="18" width="10" customWidth="1"/>
-    <col min="19" max="19" width="20" customWidth="1"/>
-    <col min="20" max="20" width="55" customWidth="1"/>
-    <col min="21" max="21" width="15" customWidth="1"/>
-    <col min="22" max="26" width="10" customWidth="1"/>
+    <col min="17" max="20" width="10" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
+    <col min="22" max="22" width="55" customWidth="1"/>
+    <col min="23" max="23" width="15" customWidth="1"/>
+    <col min="24" max="28" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="60" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" ht="60" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -736,427 +770,713 @@
         <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="G2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8">
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="V3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8">
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="8" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="9" t="s">
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="T4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="W4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8">
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="9" t="s">
+      <c r="W5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="X5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="U5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="V5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="W5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8">
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="W6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="X6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="W7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="X7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="V8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="W8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="X8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="T6" s="8" t="s">
+      <c r="P9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S9" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="V6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="W6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8">
-        <v>5</v>
+      <c r="T9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="V9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="W9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="X9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8">
+        <v>8</v>
       </c>
     </row>
-    <row r="8" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H8" s="13">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="T10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="U10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="V10" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="W10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="X10" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H12" s="11">
         <v>0</v>
       </c>
-      <c r="I8" s="14">
-        <v>1</v>
-      </c>
-      <c r="J8" s="15">
-        <v>3</v>
-      </c>
-      <c r="K8" s="16">
-        <v>1</v>
-      </c>
-      <c r="L8" s="17">
+      <c r="I12" s="12">
         <v>0</v>
       </c>
-      <c r="M8" s="18">
+      <c r="J12" s="13">
+        <v>6</v>
+      </c>
+      <c r="K12" s="14">
         <v>0</v>
       </c>
-      <c r="P8" s="13">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="14">
-        <v>1</v>
-      </c>
-      <c r="R8" s="15">
+      <c r="L12" s="15">
         <v>0</v>
       </c>
+      <c r="M12" s="16">
+        <v>0</v>
+      </c>
+      <c r="P12" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="12">
+        <v>6</v>
+      </c>
+      <c r="R12" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>54</v>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>55</v>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>56</v>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>